<commit_message>
Reload OK...need some improvement
</commit_message>
<xml_diff>
--- a/docs/Rules.xlsx
+++ b/docs/Rules.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="Task" sheetId="1" r:id="rId1"/>
     <sheet name="Exp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="97">
   <si>
     <t>TaskId</t>
   </si>
@@ -302,12 +302,21 @@
   </si>
   <si>
     <t>＊check</t>
+  </si>
+  <si>
+    <t>Reload</t>
+  </si>
+  <si>
+    <t>重新啟動</t>
+  </si>
+  <si>
+    <t>HIGH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -363,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -371,6 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +447,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -483,7 +499,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -677,7 +693,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,26 +701,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -975,7 +991,7 @@
         <v>51</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ref="O8:O29" si="1">"case TaskId."&amp;A8&amp;":"</f>
+        <f t="shared" ref="O8:O30" si="1">"case TaskId."&amp;A8&amp;":"</f>
         <v>case TaskId.DaqiaoDailyReward:</v>
       </c>
     </row>
@@ -1453,125 +1469,113 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="D23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
       <c r="O23" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.ShuangShiyiActivityReward:</v>
+        <v>case TaskId.Reload:</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" t="s">
-        <v>41</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>25</v>
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.SignIn:</v>
+        <v>case TaskId.ShuangShiyiActivityReward:</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.SLShop:</v>
+        <v>case TaskId.SignIn:</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="O26" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.StarryFight:</v>
+        <v>case TaskId.SLShop:</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>47</v>
+      <c r="F27" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>25</v>
@@ -1596,40 +1600,54 @@
       </c>
       <c r="O27" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.StarryReward:</v>
+        <v>case TaskId.StarryFight:</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="F28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="O28" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.TeamDuplicate:</v>
+        <v>case TaskId.StarryReward:</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>44</v>
@@ -1637,35 +1655,42 @@
       <c r="F29" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
       <c r="O29" t="str">
         <f t="shared" si="1"/>
-        <v>case TaskId.TrainHero:</v>
+        <v>case TaskId.TeamDuplicate:</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>49</v>
+      </c>
       <c r="E30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="O30" t="str">
+        <f t="shared" si="1"/>
+        <v>case TaskId.TrainHero:</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>51</v>
@@ -1674,16 +1699,16 @@
       <c r="E31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>47</v>
+      <c r="F31" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>51</v>
@@ -1693,6 +1718,24 @@
         <v>44</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1774,7 +1817,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f t="shared" ref="B8:C25" si="0">B7+50</f>
+        <f t="shared" ref="B8:B21" si="0">B7+50</f>
         <v>350</v>
       </c>
       <c r="C8">
@@ -2110,7 +2153,7 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
-        <f t="shared" ref="B42:C49" si="2">B41+1000</f>
+        <f t="shared" ref="B42:B49" si="2">B41+1000</f>
         <v>8000</v>
       </c>
       <c r="C42">

</xml_diff>

<commit_message>
Testing button for newton.json
</commit_message>
<xml_diff>
--- a/docs/Rules.xlsx
+++ b/docs/Rules.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
-    <sheet name="TrainHero" sheetId="2" r:id="rId2"/>
-    <sheet name="Campign" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="TrainHero" sheetId="2" r:id="rId3"/>
+    <sheet name="Campign" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Task!$A$1:$P$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Task!$A$1:$P$37</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="178">
   <si>
     <t>TaskId</t>
   </si>
@@ -405,12 +406,165 @@
   </si>
   <si>
     <t>Starry</t>
+  </si>
+  <si>
+    <t>開</t>
+  </si>
+  <si>
+    <t>關羽</t>
+  </si>
+  <si>
+    <t>黃忠</t>
+  </si>
+  <si>
+    <t>荀攸</t>
+  </si>
+  <si>
+    <t>龐統</t>
+  </si>
+  <si>
+    <t>陸遜</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>驚</t>
+  </si>
+  <si>
+    <t>孫策</t>
+  </si>
+  <si>
+    <t>夏候惇</t>
+  </si>
+  <si>
+    <t>于禁</t>
+  </si>
+  <si>
+    <t>魯肅</t>
+  </si>
+  <si>
+    <t>甄姬</t>
+  </si>
+  <si>
+    <t>杜</t>
+  </si>
+  <si>
+    <t>蔡文姬</t>
+  </si>
+  <si>
+    <t>諸葛亮</t>
+  </si>
+  <si>
+    <t>曹仁</t>
+  </si>
+  <si>
+    <t>司馬懿</t>
+  </si>
+  <si>
+    <t>徐庶</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>死</t>
+  </si>
+  <si>
+    <t>呂綺玲</t>
+  </si>
+  <si>
+    <t>張遼</t>
+  </si>
+  <si>
+    <t>周泰</t>
+  </si>
+  <si>
+    <t>典偉</t>
+  </si>
+  <si>
+    <t>呂蒙</t>
+  </si>
+  <si>
+    <t>景</t>
+  </si>
+  <si>
+    <t>休</t>
+  </si>
+  <si>
+    <t>鐘會</t>
+  </si>
+  <si>
+    <t>呂布</t>
+  </si>
+  <si>
+    <t>文醜</t>
+  </si>
+  <si>
+    <t>夏侯淵</t>
+  </si>
+  <si>
+    <t>龐德</t>
+  </si>
+  <si>
+    <t>黃月英</t>
+  </si>
+  <si>
+    <t>周瑜</t>
+  </si>
+  <si>
+    <t>馬超</t>
+  </si>
+  <si>
+    <t>大喬</t>
+  </si>
+  <si>
+    <t>孫尚香</t>
+  </si>
+  <si>
+    <t>生</t>
+  </si>
+  <si>
+    <t>太史慈</t>
+  </si>
+  <si>
+    <t>趙雲</t>
+  </si>
+  <si>
+    <t>貂蟬</t>
+  </si>
+  <si>
+    <t>張郃</t>
+  </si>
+  <si>
+    <t>華雄</t>
+  </si>
+  <si>
+    <t>賈詡</t>
+  </si>
+  <si>
+    <t>甘寧</t>
+  </si>
+  <si>
+    <t>小喬</t>
+  </si>
+  <si>
+    <t>徐晃</t>
+  </si>
+  <si>
+    <t>僇</t>
+  </si>
+  <si>
+    <t>Trials</t>
+  </si>
+  <si>
+    <t>英雄試練</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,7 +582,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +619,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -478,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -490,6 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,7 +957,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -804,26 +965,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -913,7 +1074,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="R2" t="str">
-        <f t="shared" ref="R2:R11" si="0">"case TaskId."&amp;D2&amp;":"</f>
+        <f>"case TaskId."&amp;D2&amp;":"</f>
         <v>case TaskId.Reload:</v>
       </c>
     </row>
@@ -946,7 +1107,7 @@
         <v>46</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D3&amp;":"</f>
         <v>case TaskId.MonthSignIn:</v>
       </c>
     </row>
@@ -995,7 +1156,7 @@
         <v>106</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D4&amp;":"</f>
         <v>case TaskId.FeastHero:</v>
       </c>
     </row>
@@ -1137,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D7&amp;":"</f>
         <v>case TaskId.Harvest:</v>
       </c>
     </row>
@@ -1189,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D8&amp;":"</f>
         <v>case TaskId.CleanUpBag:</v>
       </c>
     </row>
@@ -1241,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="R9" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D9&amp;":"</f>
         <v>case TaskId.CorpsCityReward:</v>
       </c>
     </row>
@@ -1293,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D10&amp;":"</f>
         <v>case TaskId.FinishTask:</v>
       </c>
     </row>
@@ -1345,7 +1506,7 @@
         <v>60</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="0"/>
+        <f>"case TaskId."&amp;D11&amp;":"</f>
         <v>case TaskId.LuckyCycle:</v>
       </c>
     </row>
@@ -1417,7 +1578,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>101</v>
@@ -1426,13 +1587,10 @@
         <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
@@ -1441,10 +1599,35 @@
       <c r="I14" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="J14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" t="str">
+        <f>"case TaskId."&amp;D14&amp;":"</f>
+        <v>case TaskId.StarryReward:</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>101</v>
@@ -1453,10 +1636,13 @@
         <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>63</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
@@ -1465,35 +1651,10 @@
       <c r="I15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R15" t="str">
-        <f>"case TaskId."&amp;D15&amp;":"</f>
-        <v>case TaskId.StarryReward:</v>
-      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>101</v>
@@ -1518,7 +1679,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>101</v>
@@ -1628,28 +1789,18 @@
         <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="R20" t="str">
         <f>"case TaskId."&amp;D20&amp;":"</f>
-        <v>case TaskId.TeamDuplicate:</v>
+        <v>case TaskId.Trials:</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1660,10 +1811,10 @@
         <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
@@ -1672,30 +1823,16 @@
       <c r="I21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="1">
-        <v>30</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O21" s="1">
-        <v>3</v>
-      </c>
-      <c r="P21" s="1">
-        <v>1</v>
-      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
       <c r="R21" t="str">
         <f>"case TaskId."&amp;D21&amp;":"</f>
-        <v>case TaskId.Patrol:</v>
+        <v>case TaskId.TeamDuplicate:</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1706,13 +1843,10 @@
         <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
@@ -1730,21 +1864,21 @@
       <c r="L22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>24</v>
+      <c r="M22" s="1">
+        <v>30</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="1">
+        <v>3</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1</v>
       </c>
       <c r="R22" t="str">
         <f>"case TaskId."&amp;D22&amp;":"</f>
-        <v>case TaskId.EliteFight:</v>
+        <v>case TaskId.Patrol:</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1755,10 +1889,10 @@
         <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="F23" t="s">
         <v>80</v>
@@ -1767,11 +1901,11 @@
       <c r="H23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>43</v>
+      <c r="I23" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>24</v>
@@ -1782,18 +1916,18 @@
       <c r="M23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O23" s="1">
-        <v>12</v>
-      </c>
-      <c r="P23" s="1">
-        <v>60</v>
+      <c r="N23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="R23" t="str">
         <f>"case TaskId."&amp;D23&amp;":"</f>
-        <v>case TaskId.GrassArrow:</v>
+        <v>case TaskId.EliteFight:</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1804,24 +1938,45 @@
         <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>47</v>
+      <c r="I24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="1">
+        <v>12</v>
+      </c>
+      <c r="P24" s="1">
+        <v>60</v>
       </c>
       <c r="R24" t="str">
         <f>"case TaskId."&amp;D24&amp;":"</f>
-        <v>case TaskId.NavalWar:</v>
+        <v>case TaskId.GrassArrow:</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -1832,10 +1987,10 @@
         <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>50</v>
@@ -1847,6 +2002,10 @@
       <c r="I25" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="R25" t="str">
+        <f>"case TaskId."&amp;D25&amp;":"</f>
+        <v>case TaskId.NavalWar:</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1856,10 +2015,10 @@
         <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>50</v>
@@ -1871,10 +2030,6 @@
       <c r="I26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R26" t="str">
-        <f t="shared" ref="R26:R36" si="1">"case TaskId."&amp;D26&amp;":"</f>
-        <v>case TaskId.SLShop:</v>
-      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1884,10 +2039,10 @@
         <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>50</v>
@@ -1900,22 +2055,22 @@
         <v>47</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.IndustryShop:</v>
+        <f>"case TaskId."&amp;D27&amp;":"</f>
+        <v>case TaskId.SLShop:</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
         <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>50</v>
@@ -1927,47 +2082,23 @@
       <c r="I28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N28" t="s">
-        <v>40</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="R28" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.Market:</v>
+        <f>"case TaskId."&amp;D28&amp;":"</f>
+        <v>case TaskId.IndustryShop:</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" t="s">
-        <v>101</v>
+      <c r="A29">
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>101</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>50</v>
@@ -1977,55 +2108,56 @@
         <v>43</v>
       </c>
       <c r="I29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" t="s">
+        <v>40</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R29" t="str">
+        <f>"case TaskId."&amp;D29&amp;":"</f>
+        <v>case TaskId.CycleShop:</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="J29" t="s">
-        <v>35</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M29" t="s">
-        <v>38</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R29" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.BossWar:</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>24</v>
+      <c r="I30" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>24</v>
@@ -2049,44 +2181,68 @@
         <v>24</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.SignIn -&gt; MonthSignIn:</v>
+        <f>"case TaskId."&amp;D30&amp;":"</f>
+        <v>case TaskId.Market:</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27</v>
+      </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I31" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.ArenaReward:</v>
+        <f>"case TaskId."&amp;D31&amp;":"</f>
+        <v>case TaskId.StarryFight:</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
         <v>25</v>
-      </c>
-      <c r="C32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>3</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>50</v>
@@ -2096,82 +2252,110 @@
         <v>43</v>
       </c>
       <c r="I32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M32" t="s">
+        <v>38</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" t="str">
+        <f>"case TaskId."&amp;D32&amp;":"</f>
+        <v>case TaskId.BossWar:</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J32" t="s">
-        <v>23</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N32" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" t="s">
         <v>40</v>
       </c>
-      <c r="O32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R32" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.CycleShop:</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F33" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" t="s">
-        <v>95</v>
+      <c r="O33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.DaqiaoDailyReward:</v>
+        <f>"case TaskId."&amp;D33&amp;":"</f>
+        <v>case TaskId.SignIn -&gt; MonthSignIn:</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>50</v>
-      </c>
-      <c r="G34" t="s">
-        <v>95</v>
-      </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
       <c r="R34" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.OneYearSignIn:</v>
+        <f>"case TaskId."&amp;D34&amp;":"</f>
+        <v>case TaskId.ArenaReward:</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="F35" t="s">
         <v>50</v>
@@ -2180,56 +2364,55 @@
         <v>95</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="1"/>
+        <f>"case TaskId."&amp;D35&amp;":"</f>
+        <v>case TaskId.DaqiaoDailyReward:</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" t="s">
+        <v>95</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="R36" t="str">
+        <f>"case TaskId."&amp;D36&amp;":"</f>
+        <v>case TaskId.OneYearSignIn:</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>95</v>
+      </c>
+      <c r="R37" t="str">
+        <f>"case TaskId."&amp;D37&amp;":"</f>
         <v>case TaskId.ShuangShiyiActivityReward:</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>26</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R36" t="str">
-        <f t="shared" si="1"/>
-        <v>case TaskId.StarryFight:</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:R33">
-    <sortCondition ref="A2:A33"/>
+  <sortState ref="A2:R36">
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
@@ -2237,6 +2420,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" t="s">
+        <v>159</v>
+      </c>
+      <c r="I6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F99"/>
   <sheetViews>
@@ -3092,7 +3474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E12"/>
   <sheetViews>
@@ -3102,9 +3484,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.125" customWidth="1"/>
+    <col min="4" max="5" width="25.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>